<commit_message>
making RAP run again
</commit_message>
<xml_diff>
--- a/RAP4/src/RAP4.xlsx
+++ b/RAP4/src/RAP4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA2C5E2-ADE2-4F5E-A4CC-47CF8CDA9DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC4DC36-A591-A64C-B7A5-7AA18085EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
   <si>
     <t>Organization</t>
   </si>
@@ -245,13 +248,37 @@
   </si>
   <si>
     <t>Type Checker</t>
+  </si>
+  <si>
+    <t>Role_Tutor</t>
+  </si>
+  <si>
+    <t>Role_AccountManager</t>
+  </si>
+  <si>
+    <t>Role_Anonymous</t>
+  </si>
+  <si>
+    <t>Role_ExecEngine</t>
+  </si>
+  <si>
+    <t>Role_Janitor</t>
+  </si>
+  <si>
+    <t>Role_SYSTEM</t>
+  </si>
+  <si>
+    <t>Role_User</t>
+  </si>
+  <si>
+    <t>Anonym</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,10 +400,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -392,7 +419,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -712,24 +739,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.1640625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -746,7 +773,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -763,7 +790,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -775,7 +802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -787,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van de Wetering</v>
@@ -802,7 +829,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -814,7 +841,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -825,7 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -842,7 +869,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +882,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -867,7 +894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -875,7 +902,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -883,7 +910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -894,7 +921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -905,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1">
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -932,7 +959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1">
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -957,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="str">
         <f>IF($B17="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -986,7 +1013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -1015,7 +1042,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
         <f>IF($B19="","",CONCATENATE("Acc_",$B5))</f>
         <v>Acc_Rogier</v>
@@ -1041,7 +1068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="str">
         <f>IF($B20="","",CONCATENATE("Acc_",$B6))</f>
         <v>Acc_Jan</v>
@@ -1063,7 +1090,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="str">
         <f>IF($B21="","",CONCATENATE("Acc_",$B7))</f>
         <v>Acc_Debbie</v>
@@ -1090,7 +1117,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1101,7 +1128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1112,170 +1139,282 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="G28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="G29" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="11" t="s">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="G30" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="11" t="s">
+      <c r="G34" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D39" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B42" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C42" s="11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="11" t="s">
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="11" t="s">
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B44" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C44" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="11" t="s">
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B45" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add labels for newly added roles
</commit_message>
<xml_diff>
--- a/RAP4/src/RAP4.xlsx
+++ b/RAP4/src/RAP4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC4DC36-A591-A64C-B7A5-7AA18085EA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8504A-BC6E-44D1-A261-9091AFC55540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="420" windowWidth="43200" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>Organization</t>
   </si>
@@ -278,7 +278,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,10 +400,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -419,7 +419,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -741,22 +741,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.1640625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -790,7 +790,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -802,7 +802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -814,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van de Wetering</v>
@@ -829,7 +829,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -841,7 +841,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -852,7 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -869,7 +869,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="7" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -894,7 +894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -902,7 +902,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -910,7 +910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -921,7 +921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -932,7 +932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="1" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -959,7 +959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -984,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f>IF($B17="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -1013,7 +1013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -1042,7 +1042,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f>IF($B19="","",CONCATENATE("Acc_",$B5))</f>
         <v>Acc_Rogier</v>
@@ -1068,7 +1068,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f>IF($B20="","",CONCATENATE("Acc_",$B6))</f>
         <v>Acc_Jan</v>
@@ -1090,7 +1090,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f>IF($B21="","",CONCATENATE("Acc_",$B7))</f>
         <v>Acc_Debbie</v>
@@ -1117,7 +1117,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="11" t="s">
         <v>50</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="11" t="s">
         <v>51</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="11" t="s">
         <v>70</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="11" t="s">
         <v>71</v>
       </c>
@@ -1187,14 +1187,16 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11" t="s">
         <v>74</v>
@@ -1206,7 +1208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="11" t="s">
         <v>52</v>
       </c>
@@ -1227,14 +1229,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11" t="s">
         <v>76</v>
@@ -1246,14 +1250,16 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11" t="s">
         <v>77</v>
@@ -1265,14 +1271,16 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11" t="s">
         <v>78</v>
@@ -1284,11 +1292,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D33" s="11"/>
@@ -1302,7 +1313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="11" t="s">
         <v>54</v>
       </c>
@@ -1323,28 +1334,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="D35" s="11"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="D36" s="11"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="D37" s="11"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="D39" s="11"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="11" t="s">
         <v>61</v>
       </c>
@@ -1356,7 +1367,7 @@
       </c>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="11" t="s">
         <v>62</v>
       </c>
@@ -1368,7 +1379,7 @@
       </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="11" t="s">
         <v>64</v>
       </c>
@@ -1380,7 +1391,7 @@
       </c>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="11" t="s">
         <v>65</v>
       </c>
@@ -1392,7 +1403,7 @@
       </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
         <v>52</v>
       </c>
@@ -1404,13 +1415,13 @@
       </c>
       <c r="D46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>

</xml_diff>

<commit_message>
Improve RAP4 wrt usability, especially the Atlas
</commit_message>
<xml_diff>
--- a/RAP4/src/RAP4.xlsx
+++ b/RAP4/src/RAP4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8504A-BC6E-44D1-A261-9091AFC55540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808EB22-B879-FE4B-9C3B-CA3CEC687BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="420" windowWidth="43200" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33580" yWindow="500" windowWidth="38400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>Organization</t>
   </si>
@@ -148,24 +148,15 @@
     <t>AccountManager</t>
   </si>
   <si>
-    <t>rogiervdw</t>
-  </si>
-  <si>
     <t>Acc_Stef</t>
   </si>
   <si>
     <t>Acc_Lloyd</t>
   </si>
   <si>
-    <t>Acc_Rogier</t>
-  </si>
-  <si>
     <t>Acc_Jan</t>
   </si>
   <si>
-    <t>Acc_Debbie</t>
-  </si>
-  <si>
     <t>Saxion</t>
   </si>
   <si>
@@ -226,9 +217,6 @@
     <t>Logout</t>
   </si>
   <si>
-    <t>debs</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -247,38 +235,32 @@
     <t>welkom</t>
   </si>
   <si>
-    <t>Type Checker</t>
-  </si>
-  <si>
-    <t>Role_Tutor</t>
-  </si>
-  <si>
-    <t>Role_AccountManager</t>
-  </si>
-  <si>
-    <t>Role_Anonymous</t>
-  </si>
-  <si>
-    <t>Role_ExecEngine</t>
-  </si>
-  <si>
-    <t>Role_Janitor</t>
-  </si>
-  <si>
-    <t>Role_SYSTEM</t>
-  </si>
-  <si>
-    <t>Role_User</t>
-  </si>
-  <si>
-    <t>Anonym</t>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Edit_32_navigation_32_menu</t>
+  </si>
+  <si>
+    <t>[PF_Interface]</t>
+  </si>
+  <si>
+    <t>PF_Interface</t>
+  </si>
+  <si>
+    <t>Edit Navigation Menu</t>
+  </si>
+  <si>
+    <t>List_32_all_32_interfaces</t>
+  </si>
+  <si>
+    <t>List all interfaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,7 +346,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -385,9 +367,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -400,10 +379,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -419,7 +398,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -739,32 +718,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.1640625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2"/>
@@ -773,15 +752,15 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2"/>
@@ -790,165 +769,167 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van de Wetering</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>54</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>43</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>44</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1">
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
@@ -959,21 +940,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1">
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
@@ -984,16 +967,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="str">
         <f>IF($B17="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A3</f>
@@ -1003,6 +986,9 @@
         <f>$A$10</f>
         <v>OUNL</v>
       </c>
+      <c r="F17" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="G17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1010,26 +996,26 @@
         <v>39</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" s="7" t="str">
         <f>$A4</f>
         <v>Lloyd Rutledge</v>
       </c>
       <c r="E18" s="5" t="str">
-        <f t="shared" ref="E18:E19" si="2">$A$10</f>
+        <f t="shared" ref="E18" si="2">$A$10</f>
         <v>OUNL</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1039,393 +1025,339 @@
         <v>39</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
-        <f>IF($B19="","",CONCATENATE("Acc_",$B5))</f>
-        <v>Acc_Rogier</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>40</v>
+        <f>IF($B19="","",CONCATENATE("Acc_",$B6))</f>
+        <v>Acc_Jan</v>
+      </c>
+      <c r="B19" s="9">
+        <v>123456</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19" si="3">$A5</f>
-        <v>Rogier van de Wetering</v>
-      </c>
-      <c r="E19" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>OUNL</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="6" t="str">
-        <f>IF($B20="","",CONCATENATE("Acc_",$B6))</f>
-        <v>Acc_Jan</v>
-      </c>
-      <c r="B20" s="10">
-        <v>123456</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="7" t="str">
         <f>$A6</f>
         <v>Jan de Student</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="6" t="str">
-        <f>IF($B21="","",CONCATENATE("Acc_",$B7))</f>
-        <v>Acc_Debbie</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="5" t="str">
-        <f>$A$14</f>
-        <v>HAN</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I19" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="B22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="11" t="s">
+      <c r="B29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="11" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="11" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
+      <c r="D40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="D39" s="11"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="11" t="s">
+      <c r="D41" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="11" t="s">
+      <c r="B46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="11" t="s">
+      <c r="B47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
+      <c r="B48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
fix for a non-documented deployment bug (but the software is slightly more maintainable)
The compiler could not find html-templates added by RAP because it was looking from the wrong working directory.
</commit_message>
<xml_diff>
--- a/RAP4/src/RAP4.xlsx
+++ b/RAP4/src/RAP4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C808EB22-B879-FE4B-9C3B-CA3CEC687BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB6349-FDB7-F64C-9ED5-8DE14F37580C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33580" yWindow="500" windowWidth="38400" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="21600" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>Organization</t>
   </si>
@@ -236,24 +236,6 @@
   </si>
   <si>
     <t>Advanced</t>
-  </si>
-  <si>
-    <t>Edit_32_navigation_32_menu</t>
-  </si>
-  <si>
-    <t>[PF_Interface]</t>
-  </si>
-  <si>
-    <t>PF_Interface</t>
-  </si>
-  <si>
-    <t>Edit Navigation Menu</t>
-  </si>
-  <si>
-    <t>List_32_all_32_interfaces</t>
-  </si>
-  <si>
-    <t>List all interfaces</t>
   </si>
 </sst>
 </file>
@@ -718,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:C45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1212,23 +1194,20 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -1240,124 +1219,76 @@
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>46</v>
+      <c r="A39" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Treat property rules different from other rules in the RAP interface
</commit_message>
<xml_diff>
--- a/RAP4/src/RAP4.xlsx
+++ b/RAP4/src/RAP4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB6349-FDB7-F64C-9ED5-8DE14F37580C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ACA6EE-A75B-BC4A-81C7-8254AB2C941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="21600" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42000" yWindow="3760" windowWidth="21600" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Organization</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>ExecEngine</t>
-  </si>
-  <si>
-    <t>Janitor</t>
   </si>
   <si>
     <t>SYSTEM</t>
@@ -703,7 +700,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -784,10 +781,10 @@
         <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -799,7 +796,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -927,7 +924,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>5</v>
@@ -958,7 +955,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A3</f>
@@ -969,7 +966,7 @@
         <v>OUNL</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>27</v>
@@ -990,7 +987,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="7" t="str">
         <f>$A4</f>
@@ -1019,7 +1016,7 @@
         <v>123456</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="7" t="str">
         <f>$A6</f>
@@ -1049,7 +1046,7 @@
         <v>35</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>45</v>
@@ -1060,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>46</v>
@@ -1092,25 +1089,25 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="10"/>
     </row>
@@ -1155,10 +1152,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -1168,10 +1165,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1194,21 +1191,17 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
     </row>
@@ -1220,10 +1213,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>45</v>
@@ -1232,10 +1225,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>46</v>
@@ -1244,25 +1237,25 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" s="10"/>
     </row>

</xml_diff>